<commit_message>
updated daily cases uk
</commit_message>
<xml_diff>
--- a/data/UK/DailyConfirmedCases.xlsx
+++ b/data/UK/DailyConfirmedCases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\phe.gov.uk\porton\SharedData\ERD_Sci_Tech\GIS\PROJECTS AND INCIDENTS\Incidents\2020 Wuhan Coronavirus\AGOL\COVID19_Esri_AGOL_External\Processing\20200313\3_PRODUCTION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\phe.gov.uk\porton\SharedData\ERD_Sci_Tech\GIS\PROJECTS AND INCIDENTS\Incidents\2020 Wuhan Coronavirus\AGOL\COVID19_Esri_AGOL_External\Processing\20200314\3_PRODUCTION\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12036"/>
   </bookViews>
   <sheets>
     <sheet name="DailyConfirmedCases" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -79,14 +79,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,19 +414,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="1" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -424,477 +437,531 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43861</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
+        <f>B2</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43862</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C37" si="0">B3+C2</f>
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43863</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43864</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43865</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43866</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43867</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43868</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>43869</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43870</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>43871</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>4</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>43872</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>43873</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>43874</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>43875</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>43876</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>43877</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>43878</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>43879</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>43880</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>43881</v>
       </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>43882</v>
       </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>43883</v>
       </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>43884</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>43885</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>4</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>43886</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>43887</v>
       </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>43888</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>43889</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>6</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>43890</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>4</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>43891</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>12</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="1">
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>43892</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>5</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="1">
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>43893</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>11</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="1">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>43894</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>34</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="1">
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>43895</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>29</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="1">
+        <f t="shared" si="0"/>
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>43896</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>46</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>43897</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>46</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
+        <f>C37+B38</f>
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>43898</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>65</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
+        <f t="shared" ref="C39:C45" si="1">C38+B39</f>
         <v>271</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>43899</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>50</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
+        <f t="shared" si="1"/>
         <v>321</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>43900</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>52</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
+        <f t="shared" si="1"/>
         <v>373</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>43901</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>83</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
+        <f t="shared" si="1"/>
         <v>456</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
         <v>43902</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="4">
         <v>139</v>
       </c>
-      <c r="C43">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="1">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43903</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="4">
         <v>207</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
+        <f t="shared" si="1"/>
         <v>797</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>43904</v>
+      </c>
+      <c r="B45" s="4">
+        <v>343</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="1"/>
+        <v>1140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>